<commit_message>
finished writing main paper
</commit_message>
<xml_diff>
--- a/Basketball_dataset_clean_2.xlsx
+++ b/Basketball_dataset_clean_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jake3\Desktop\Math_Modeling_Comp\OSU-MCM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73d75a060ff8ff51/Documents/GitHub/OSU-MCM/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{50FE4782-B844-489B-AF76-D39BE0113B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="33" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teams" sheetId="1" r:id="rId1"/>
@@ -2780,16 +2780,16 @@
   </sheetPr>
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.86328125" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="5" max="5" width="42.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3565,14 +3565,14 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="20.53125" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -4422,12 +4422,12 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="17.46484375" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -5277,12 +5277,12 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="16.46484375" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -6086,7 +6086,7 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -6998,12 +6998,12 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.46484375" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" customWidth="1"/>
     <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8840,7 +8840,7 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -9663,7 +9663,7 @@
       <selection activeCell="E1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -10509,7 +10509,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -11401,7 +11401,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -12201,7 +12201,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -12905,16 +12905,16 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="20.53125" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -13879,7 +13879,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -14495,7 +14495,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -15318,7 +15318,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -16164,7 +16164,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
@@ -16916,7 +16916,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -17737,7 +17737,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -18558,7 +18558,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -19425,7 +19425,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -20269,7 +20269,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -21090,7 +21090,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -21907,13 +21907,15 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
@@ -22816,7 +22818,7 @@
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -23637,7 +23639,7 @@
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -24481,7 +24483,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -25302,7 +25304,7 @@
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -26146,7 +26148,7 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -26992,7 +26994,7 @@
       <selection activeCell="E1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -27861,7 +27863,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -28684,7 +28686,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -29507,7 +29509,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -30326,11 +30328,11 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1">
       <c r="A1" s="11" t="s">
@@ -30355,7 +30357,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.4">
+    <row r="2" spans="1:7" ht="14.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -30378,7 +30380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.4">
+    <row r="3" spans="1:7" ht="14.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -30401,7 +30403,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4">
+    <row r="4" spans="1:7" ht="14.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -30424,7 +30426,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.4">
+    <row r="5" spans="1:7" ht="14.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -30447,7 +30449,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.4">
+    <row r="6" spans="1:7" ht="14.25">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -30470,7 +30472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.4">
+    <row r="7" spans="1:7" ht="14.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -30493,7 +30495,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.4">
+    <row r="8" spans="1:7" ht="14.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -30516,7 +30518,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4">
+    <row r="9" spans="1:7" ht="14.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -30539,7 +30541,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.4">
+    <row r="10" spans="1:7" ht="14.25">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -30562,7 +30564,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.4">
+    <row r="11" spans="1:7" ht="14.25">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -30585,7 +30587,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.4">
+    <row r="12" spans="1:7" ht="14.25">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -30608,7 +30610,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.4">
+    <row r="13" spans="1:7" ht="14.25">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -30631,7 +30633,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.4">
+    <row r="14" spans="1:7" ht="14.25">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -30654,7 +30656,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.4">
+    <row r="15" spans="1:7" ht="14.25">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -30677,7 +30679,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.4">
+    <row r="16" spans="1:7" ht="14.25">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -30700,7 +30702,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.4">
+    <row r="17" spans="1:7" ht="14.25">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -30723,7 +30725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.4">
+    <row r="18" spans="1:7" ht="14.25">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -30746,7 +30748,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.4">
+    <row r="19" spans="1:7" ht="14.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -30769,7 +30771,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.4">
+    <row r="20" spans="1:7" ht="14.25">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -30792,7 +30794,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.4">
+    <row r="21" spans="1:7" ht="14.25">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -30815,7 +30817,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.4">
+    <row r="22" spans="1:7" ht="14.25">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -30838,7 +30840,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.4">
+    <row r="23" spans="1:7" ht="14.25">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -30861,7 +30863,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.4">
+    <row r="24" spans="1:7" ht="14.25">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -30884,7 +30886,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.4">
+    <row r="25" spans="1:7" ht="14.25">
       <c r="A25" s="11">
         <v>24</v>
       </c>
@@ -30907,7 +30909,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.4">
+    <row r="26" spans="1:7" ht="14.25">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -30930,7 +30932,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.4">
+    <row r="27" spans="1:7" ht="14.25">
       <c r="A27" s="11">
         <v>26</v>
       </c>
@@ -30953,7 +30955,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.4">
+    <row r="28" spans="1:7" ht="14.25">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -30976,7 +30978,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.4">
+    <row r="29" spans="1:7" ht="14.25">
       <c r="A29" s="11">
         <v>28</v>
       </c>
@@ -30999,7 +31001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.4">
+    <row r="30" spans="1:7" ht="14.25">
       <c r="A30" s="11">
         <v>29</v>
       </c>
@@ -31022,7 +31024,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="14.4">
+    <row r="31" spans="1:7" ht="14.25">
       <c r="A31" s="11">
         <v>30</v>
       </c>
@@ -31045,7 +31047,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.4">
+    <row r="32" spans="1:7" ht="14.25">
       <c r="A32" s="11">
         <v>31</v>
       </c>
@@ -31068,7 +31070,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.4">
+    <row r="33" spans="1:7" ht="14.25">
       <c r="A33" s="11">
         <v>32</v>
       </c>
@@ -31091,7 +31093,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.4">
+    <row r="34" spans="1:7" ht="14.25">
       <c r="A34" s="11">
         <v>33</v>
       </c>
@@ -31128,11 +31130,11 @@
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
@@ -32075,7 +32077,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -32967,7 +32969,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -33813,7 +33815,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -34636,7 +34638,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -35505,7 +35507,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -36374,7 +36376,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
@@ -37243,7 +37245,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -38227,7 +38229,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -39119,7 +39121,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -39965,7 +39967,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -40832,12 +40834,12 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -41733,7 +41735,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -42556,7 +42558,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -43402,7 +43404,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -44248,7 +44250,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -45048,7 +45050,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -45894,7 +45896,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -46740,7 +46742,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -47609,7 +47611,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -48455,7 +48457,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -49301,7 +49303,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -50145,12 +50147,12 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="17.46484375" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -51023,7 +51025,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -51892,7 +51894,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -52715,7 +52717,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -53561,7 +53563,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -54359,12 +54361,12 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="23.86328125" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -55214,7 +55216,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -56060,7 +56062,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -56906,7 +56908,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -57796,7 +57798,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -58642,7 +58644,7 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -59440,11 +59442,11 @@
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
@@ -60314,14 +60316,16 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
@@ -61215,12 +61219,12 @@
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="21.53125" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>

</xml_diff>

<commit_message>
Elo, Histogram, Upset %'s
</commit_message>
<xml_diff>
--- a/Basketball_dataset_clean_2.xlsx
+++ b/Basketball_dataset_clean_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jake3\Desktop\Math_Modeling_Comp\OSU-MCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{395A7D85-5D65-4C66-B686-B495B6F52A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EE85E9-8CEA-43F5-87C7-277882E76BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="65" activeTab="66" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teams" sheetId="1" r:id="rId1"/>
@@ -2613,10 +2613,10 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2840,8 +2840,8 @@
   </sheetPr>
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -12257,8 +12257,8 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="A38" sqref="A30:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -14119,8 +14119,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -55713,7 +55713,7 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
@@ -56559,7 +56559,7 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
@@ -57405,8 +57405,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -59920,7 +59920,9 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>